<commit_message>
Upgrade example Excel file.
</commit_message>
<xml_diff>
--- a/ExcelCli/Character.xlsx
+++ b/ExcelCli/Character.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\ExcelToDotnet\ExcelCli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1F832E-1ACE-43FA-AB47-99385FE3F6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E89B8D-7407-4310-A037-56184F3538CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25995" windowHeight="20985" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17940" yWindow="345" windowWidth="24150" windowHeight="13080" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="3" r:id="rId1"/>
-    <sheet name="ConstLobby" sheetId="16" r:id="rId2"/>
-    <sheet name="Character" sheetId="7" r:id="rId3"/>
-    <sheet name="CharacterStat" sheetId="12" r:id="rId4"/>
-    <sheet name="Prob" sheetId="17" r:id="rId5"/>
-    <sheet name="Sub" sheetId="18" r:id="rId6"/>
+    <sheet name="Comment" sheetId="20" r:id="rId2"/>
+    <sheet name="Vector" sheetId="22" r:id="rId3"/>
+    <sheet name="!Lobby" sheetId="21" r:id="rId4"/>
+    <sheet name="ConstLobby" sheetId="16" r:id="rId5"/>
+    <sheet name="Character" sheetId="7" r:id="rId6"/>
+    <sheet name="CharacterStat" sheetId="12" r:id="rId7"/>
+    <sheet name="Prob" sheetId="17" r:id="rId8"/>
+    <sheet name="Sub" sheetId="18" r:id="rId9"/>
+    <sheet name="# 주석 시트" sheetId="19" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
   <si>
     <t>Hp</t>
   </si>
@@ -100,14 +104,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Id</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>DateTime</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -296,6 +292,46 @@
   </si>
   <si>
     <t>서브인덱스</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t># Comment Column (주석 열)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t># Comment Row (주석 행)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vector3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>!Vector3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1,2,3&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;2,3,4&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vector2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>!Vector2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;2,3&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1,2&gt;</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -385,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +443,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -440,7 +482,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -462,6 +504,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="보통" xfId="1" builtinId="28"/>
@@ -760,42 +805,42 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,77 +911,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775CC093-F05D-4AA7-9DAF-63CBCF88DDB8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8E5896-93BB-4CCB-ACE5-80205C60553D}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -945,11 +1039,243 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D86FF33-1701-4233-AB32-42D2888EBBEC}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A4DC4B-0799-4470-AC7D-CBE06B38CE78}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -976,48 +1302,48 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1028,19 +1354,19 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
@@ -1048,39 +1374,39 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="14">
         <v>0.25638888888888889</v>
@@ -1089,7 +1415,7 @@
         <v>0.25638888888888889</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="3" t="s">
@@ -1098,7 +1424,7 @@
     </row>
     <row r="6" spans="1:9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1110,23 +1436,23 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="14">
         <v>0.25638888888888889</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>13</v>
@@ -1134,7 +1460,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1144,12 +1470,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1183,12 +1509,12 @@
         <v>4</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>46</v>
+      <c r="A2" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1208,27 +1534,27 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>200</v>
@@ -1248,7 +1574,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>300</v>
@@ -1268,7 +1594,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1283,7 +1609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0868C69-F2AE-42B5-9525-2D7336E703C6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1301,33 +1627,33 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3">
         <v>60</v>
@@ -1336,7 +1662,7 @@
     </row>
     <row r="5" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3">
         <v>40</v>
@@ -1345,7 +1671,7 @@
     </row>
     <row r="6" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="1"/>
@@ -1357,12 +1683,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348BF195-9DCA-48BF-A378-E29241F0ABAD}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1376,66 +1702,66 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>

</xml_diff>

<commit_message>
fixed only string column validate id. (changes check all column type)
</commit_message>
<xml_diff>
--- a/ExcelCli/Character.xlsx
+++ b/ExcelCli/Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\ExcelToDotnet\ExcelCli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E89B8D-7407-4310-A037-56184F3538CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90408127-DEE9-45DD-8298-C8B2E123E22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17940" yWindow="345" windowWidth="24150" windowHeight="13080" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="25995" windowHeight="20985" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>Hp</t>
   </si>
@@ -251,10 +251,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>%percent</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -332,6 +328,22 @@
   </si>
   <si>
     <t>&lt;1,2&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroupId</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>%GroupId</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -915,12 +927,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775CC093-F05D-4AA7-9DAF-63CBCF88DDB8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -949,7 +962,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>53</v>
@@ -1002,7 +1015,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1060,10 +1073,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>53</v>
@@ -1071,16 +1084,16 @@
     </row>
     <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -1107,10 +1120,10 @@
         <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1122,10 +1135,10 @@
         <v>48</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1611,70 +1624,108 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0868C69-F2AE-42B5-9525-2D7336E703C6}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="3">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="3">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="1"/>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1688,7 +1739,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1702,10 +1753,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>53</v>
@@ -1713,13 +1764,13 @@
     </row>
     <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -1737,25 +1788,25 @@
     </row>
     <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1"/>
     </row>

</xml_diff>

<commit_message>
added string value Trim().
</commit_message>
<xml_diff>
--- a/ExcelCli/Character.xlsx
+++ b/ExcelCli/Character.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\ExcelToDotnet\ExcelCli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90408127-DEE9-45DD-8298-C8B2E123E22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC14B1F9-10C2-4AE7-8D0D-8DE946EBE317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25995" windowHeight="20985" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25650" yWindow="0" windowWidth="26055" windowHeight="20985" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="3" r:id="rId1"/>
@@ -196,10 +196,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>List&lt;CharacterType&gt;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Enum 목록</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -344,6 +340,10 @@
   </si>
   <si>
     <t>%GroupId</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;CharacterType?&gt;</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -817,13 +817,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -962,10 +962,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
@@ -985,16 +985,16 @@
     </row>
     <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1003,7 +1003,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>16</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1026,7 +1026,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="7" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1073,42 +1073,42 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1117,13 +1117,13 @@
         <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1132,19 +1132,19 @@
         <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1176,7 +1176,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.2">
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1330,18 +1330,18 @@
         <v>14</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>27</v>
@@ -1367,7 +1367,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -1387,28 +1387,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,10 +1416,10 @@
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="14">
         <v>0.25638888888888889</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="6" spans="1:9" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1452,10 +1452,10 @@
         <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="14">
         <v>0.25638888888888889</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1522,12 +1522,12 @@
         <v>4</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1547,22 +1547,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1626,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0868C69-F2AE-42B5-9525-2D7336E703C6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1641,42 +1641,42 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="7" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="8" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7"/>
     </row>
@@ -1753,66 +1753,66 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>

</xml_diff>